<commit_message>
bi: update oncho form
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Senegal/2023/jul 2023/sn_lf_pretas_2_partcipants_202307.xlsx
+++ b/LF/PreTAS/Senegal/2023/jul 2023/sn_lf_pretas_2_partcipants_202307.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\PreTAS\Senegal\2023\jul 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D647D4-159A-483B-AA08-1D48A151E1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B175E4CF-D391-49BB-812E-3515C0ED6051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="107">
   <si>
     <t>type</t>
   </si>
@@ -328,9 +328,6 @@
   </si>
   <si>
     <t>p_GenerateID</t>
-  </si>
-  <si>
-    <t>${p_IDMethod} = 'ID_generation' and ${p_consent} = 'Yes'</t>
   </si>
   <si>
     <t>concat(${p_cluster_id},'-',substr(random(),3,10))</t>
@@ -818,7 +815,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1193,7 +1190,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L11" s="14"/>
       <c r="M11" s="15" t="s">
@@ -1223,10 +1220,10 @@
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
       <c r="K12" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L12" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M12" s="15" t="s">
         <v>25</v>
@@ -1523,10 +1520,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>92</v>

</xml_diff>